<commit_message>
result_path 버튼 삭제 전
</commit_message>
<xml_diff>
--- a/root/result.xlsx
+++ b/root/result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D164"/>
+  <dimension ref="A1:F167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,2631 +434,3635 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Hyperparameter Batch size = 4, Learning rate = 2e-4, optimizer = adam, aug = 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>landmark_num</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>landmark_name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
         <is>
           <t>aver</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0.8694895053995684</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.8694895053995684</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Sella</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0.1212435565298096</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.1212435565298096</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>R FZP</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0.1056550992617137</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.1056550992617137</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>L FZP</t>
+          <t>N</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.056550992617039</v>
+        <v>5.196152422706632</v>
       </c>
       <c r="D5" t="n">
-        <v>1.056550992617039</v>
+        <v>12.12435565298214</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8.660254037844387</v>
+      </c>
+      <c r="F5" t="n">
+        <v>8.660254037844387</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R Or</t>
+          <t>Sella</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.01905255888325017</v>
+        <v>3.464101615137754</v>
       </c>
       <c r="D6" t="n">
-        <v>0.01905255888325017</v>
+        <v>12.12435565298214</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.464101615137754</v>
+      </c>
+      <c r="F6" t="n">
+        <v>6.350852961085883</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>L Or</t>
+          <t>R FZP</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.1593486742963099</v>
+        <v>5.196152422706632</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1593486742963099</v>
+        <v>10.39230484541326</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5.196152422706632</v>
+      </c>
+      <c r="F7" t="n">
+        <v>6.928203230275508</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R Po</t>
+          <t>L FZP</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.04330127018921947</v>
+        <v>1.056550992617039</v>
       </c>
       <c r="D8" t="n">
-        <v>0.04330127018921947</v>
+        <v>1.056550992617039</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.056550992617039</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.056550992617039</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>L Po</t>
+          <t>R Or</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.853901048131497</v>
+        <v>0.01905255888325017</v>
       </c>
       <c r="D9" t="n">
-        <v>0.853901048131497</v>
+        <v>0.01905255888325017</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.01905255888325017</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.01905255888325017</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R TFP</t>
+          <t>L Or</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.07447818472546044</v>
+        <v>0.1593486742963099</v>
       </c>
       <c r="D10" t="n">
-        <v>0.07447818472546044</v>
+        <v>0.1593486742963099</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.1593486742963099</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.1593486742963099</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>L TFP</t>
+          <t>R Po</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2856.151781681079</v>
+        <v>0.04330127018921947</v>
       </c>
       <c r="D11" t="n">
-        <v>2856.151781681079</v>
+        <v>0.04330127018921947</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.04330127018921947</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.04330127018921947</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R KRP</t>
+          <t>L Po</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.1524204710660506</v>
+        <v>0.853901048131497</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1524204710660506</v>
+        <v>0.853901048131497</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.853901048131497</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.853901048131497</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>L KRP</t>
+          <t>R TFP</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2513.205721782441</v>
+        <v>0.07447818472546044</v>
       </c>
       <c r="D13" t="n">
-        <v>2513.205721782441</v>
+        <v>0.07447818472546044</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.07447818472546044</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.07447818472546044</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ANS</t>
+          <t>L TFP</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1827.313601985166</v>
+        <v>2856.151781681079</v>
       </c>
       <c r="D14" t="n">
-        <v>1827.313601985166</v>
+        <v>2856.151781681079</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2856.151781681079</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2856.151781681079</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>15</v>
+        <v>125</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>PNS</t>
+          <t>R KRP</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1827.313601985166</v>
+        <v>0.1524204710660506</v>
       </c>
       <c r="D15" t="n">
-        <v>1827.313601985166</v>
+        <v>969.9484522385712</v>
+      </c>
+      <c r="E15" t="n">
+        <v>969.9484522385712</v>
+      </c>
+      <c r="F15" t="n">
+        <v>646.6831083160695</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>18</v>
+        <v>126</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>L KRP</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1827.313601985166</v>
+        <v>2513.205721782441</v>
       </c>
       <c r="D16" t="n">
-        <v>1827.313601985166</v>
+        <v>829.6523368254922</v>
+      </c>
+      <c r="E16" t="n">
+        <v>829.6523368254922</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1390.836798477809</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>19</v>
+        <v>128</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>ANS</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1811.725144717046</v>
+        <v>1827.313601985166</v>
       </c>
       <c r="D17" t="n">
-        <v>1811.725144717046</v>
+        <v>1110.24456765165</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1110.24456765165</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1349.267579096155</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Pog</t>
+          <t>PNS</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1796.136687448926</v>
+        <v>1827.313601985166</v>
       </c>
       <c r="D18" t="n">
-        <v>1796.136687448926</v>
+        <v>969.9484522385712</v>
+      </c>
+      <c r="E18" t="n">
+        <v>969.9484522385712</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1255.736835487436</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Gn</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1796.136687448926</v>
+        <v>1827.313601985166</v>
       </c>
       <c r="D19" t="n">
-        <v>1796.136687448926</v>
+        <v>985.5369095066911</v>
+      </c>
+      <c r="E19" t="n">
+        <v>985.5369095066911</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1266.129140332849</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Me</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1796.136687448926</v>
+        <v>1811.725144717046</v>
       </c>
       <c r="D20" t="n">
-        <v>1796.136687448926</v>
+        <v>923.1830804342115</v>
+      </c>
+      <c r="E20" t="n">
+        <v>923.1830804342115</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1219.36376852849</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>28</v>
+        <v>135</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>R CP Point</t>
+          <t>Pog</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1.009785620812653</v>
+        <v>1796.136687448926</v>
       </c>
       <c r="D21" t="n">
-        <v>1.009785620812653</v>
+        <v>969.9484522385712</v>
+      </c>
+      <c r="E21" t="n">
+        <v>969.9484522385712</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1245.344530642023</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>29</v>
+        <v>139</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>L CP Point</t>
+          <t>Gn</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2575.55955085492</v>
+        <v>1796.136687448926</v>
       </c>
       <c r="D22" t="n">
-        <v>2575.55955085492</v>
+        <v>2684.67875173176</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2684.67875173176</v>
+      </c>
+      <c r="F22" t="n">
+        <v>2388.498063637482</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>32</v>
+        <v>140</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>R Sigmoid notch</t>
+          <t>Me</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.02771281292108668</v>
+        <v>1796.136687448926</v>
       </c>
       <c r="D23" t="n">
-        <v>0.02771281292108668</v>
+        <v>2684.67875173176</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2684.67875173176</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2388.498063637482</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>L Sigmoid notch</t>
+          <t>R CP Point</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2591.148008123041</v>
+        <v>1.009785620812653</v>
       </c>
       <c r="D24" t="n">
-        <v>2591.148008123041</v>
+        <v>2528.794179050561</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2528.794179050561</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1686.199381240645</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>R Anterior ramal point</t>
+          <t>L CP Point</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1.072139449885135</v>
+        <v>2575.55955085492</v>
       </c>
       <c r="D25" t="n">
-        <v>1.072139449885135</v>
+        <v>2684.67875173176</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2684.67875173176</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2648.305684772813</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>35</v>
+        <v>146</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>L Anterior ramal point</t>
+          <t>R Sigmoid notch</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2482.028807246201</v>
+        <v>0.02771281292108668</v>
       </c>
       <c r="D26" t="n">
-        <v>2482.028807246201</v>
+        <v>2684.67875173176</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2684.67875173176</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1789.795072092147</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>36</v>
+        <v>147</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>R Post Go</t>
+          <t>L Sigmoid notch</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.635662646377761</v>
+        <v>2591.148008123041</v>
       </c>
       <c r="D27" t="n">
-        <v>0.635662646377761</v>
+        <v>2684.67875173176</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2684.67875173176</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2653.50183719552</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>37</v>
+        <v>148</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>L Post Go</t>
+          <t>R Anterior ramal point</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2544.382636318681</v>
+        <v>1.072139449885135</v>
       </c>
       <c r="D28" t="n">
-        <v>2544.382636318681</v>
+        <v>2684.67875173176</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2684.67875173176</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1790.143214304468</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>R Go</t>
+          <t>L Anterior ramal point</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.4018357873559784</v>
+        <v>2482.028807246201</v>
       </c>
       <c r="D29" t="n">
-        <v>0.4018357873559784</v>
+        <v>814.0638795573723</v>
+      </c>
+      <c r="E29" t="n">
+        <v>814.0638795573723</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1370.052188786982</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>L Go</t>
+          <t>R Post Go</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>2513.205721782441</v>
+        <v>0.635662646377761</v>
       </c>
       <c r="D30" t="n">
-        <v>2513.205721782441</v>
+        <v>1188.18685399225</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1188.18685399225</v>
+      </c>
+      <c r="F30" t="n">
+        <v>792.3364568769592</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>R Inf Go</t>
+          <t>L Post Go</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1.087727907153255</v>
+        <v>2544.382636318681</v>
       </c>
       <c r="D31" t="n">
-        <v>1.087727907153255</v>
+        <v>969.9484522385712</v>
+      </c>
+      <c r="E31" t="n">
+        <v>969.9484522385712</v>
+      </c>
+      <c r="F31" t="n">
+        <v>1494.759846931941</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>L Inf Go</t>
+          <t>R Go</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2497.617264514321</v>
+        <v>0.4018357873559784</v>
       </c>
       <c r="D32" t="n">
-        <v>2497.617264514321</v>
+        <v>1001.125366774811</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1001.125366774811</v>
+      </c>
+      <c r="F32" t="n">
+        <v>667.5508564456594</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>42</v>
+        <v>137</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>U1MP</t>
+          <t>L Go</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1827.313601985166</v>
+        <v>2513.205721782441</v>
       </c>
       <c r="D33" t="n">
-        <v>1827.313601985166</v>
+        <v>923.1830804342115</v>
+      </c>
+      <c r="E33" t="n">
+        <v>923.1830804342115</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1453.190627550288</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>R U1CP</t>
+          <t>R Inf Go</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1764.959772912686</v>
+        <v>1.087727907153255</v>
       </c>
       <c r="D34" t="n">
-        <v>1764.959772912686</v>
+        <v>969.9484522385712</v>
+      </c>
+      <c r="E34" t="n">
+        <v>969.9484522385712</v>
+      </c>
+      <c r="F34" t="n">
+        <v>646.9948774614319</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>44</v>
+        <v>143</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>R U1RP</t>
+          <t>L Inf Go</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1780.548230180806</v>
+        <v>2497.617264514321</v>
       </c>
       <c r="D35" t="n">
-        <v>1780.548230180806</v>
+        <v>2840.563324412959</v>
+      </c>
+      <c r="E35" t="n">
+        <v>2840.563324412959</v>
+      </c>
+      <c r="F35" t="n">
+        <v>2726.247971113413</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>45</v>
+        <v>144</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>L U1CP</t>
+          <t>U1MP</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1889.667431057645</v>
+        <v>1827.313601985166</v>
       </c>
       <c r="D36" t="n">
-        <v>1889.667431057645</v>
+        <v>2372.909606369362</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2372.909606369362</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2191.04427157463</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>L U1RP</t>
+          <t>R U1CP</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1874.078973789525</v>
+        <v>1764.959772912686</v>
       </c>
       <c r="D37" t="n">
-        <v>1874.078973789525</v>
+        <v>2684.67875173176</v>
+      </c>
+      <c r="E37" t="n">
+        <v>2684.67875173176</v>
+      </c>
+      <c r="F37" t="n">
+        <v>2378.105758792069</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>R U3CP</t>
+          <t>R U1RP</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.9162548772039298</v>
+        <v>1780.548230180806</v>
       </c>
       <c r="D38" t="n">
-        <v>0.9162548772039298</v>
+        <v>2528.794179050561</v>
+      </c>
+      <c r="E38" t="n">
+        <v>2528.794179050561</v>
+      </c>
+      <c r="F38" t="n">
+        <v>2279.378862760643</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>R U3RP</t>
+          <t>L U1CP</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1577.898285695247</v>
+        <v>1889.667431057645</v>
       </c>
       <c r="D39" t="n">
-        <v>1577.898285695247</v>
+        <v>2684.67875173176</v>
+      </c>
+      <c r="E39" t="n">
+        <v>2684.67875173176</v>
+      </c>
+      <c r="F39" t="n">
+        <v>2419.674978173721</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>L U3CP</t>
+          <t>L U1RP</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>2123.494290079444</v>
+        <v>1874.078973789525</v>
       </c>
       <c r="D40" t="n">
-        <v>2123.494290079444</v>
+        <v>2684.67875173176</v>
+      </c>
+      <c r="E40" t="n">
+        <v>2684.67875173176</v>
+      </c>
+      <c r="F40" t="n">
+        <v>2414.478825751015</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>L U3RP</t>
+          <t>R U3CP</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2061.140461006964</v>
+        <v>0.9162548772039298</v>
       </c>
       <c r="D41" t="n">
-        <v>2061.140461006964</v>
+        <v>0.1524204710660506</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.1524204710660506</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.407031939778677</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>R U6CP</t>
+          <t>R U3RP</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.1905255888325755</v>
+        <v>1577.898285695247</v>
       </c>
       <c r="D42" t="n">
-        <v>0.1905255888325755</v>
+        <v>2513.205721782441</v>
+      </c>
+      <c r="E42" t="n">
+        <v>2513.205721782441</v>
+      </c>
+      <c r="F42" t="n">
+        <v>2201.436576420043</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>R U6RP</t>
+          <t>L U3CP</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.2684678751731779</v>
+        <v>2123.494290079444</v>
       </c>
       <c r="D43" t="n">
-        <v>0.2684678751731779</v>
+        <v>1827.313601985166</v>
+      </c>
+      <c r="E43" t="n">
+        <v>1827.313601985166</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1926.040498016592</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>L U6CP</t>
+          <t>L U3RP</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>2232.613490956283</v>
+        <v>2061.140461006964</v>
       </c>
       <c r="D44" t="n">
-        <v>2232.613490956283</v>
+        <v>1827.313601985166</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1827.313601985166</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1905.255888325765</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>L U6RP</t>
+          <t>R U6CP</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>2232.613490956283</v>
+        <v>0.1905255888325755</v>
       </c>
       <c r="D45" t="n">
-        <v>2232.613490956283</v>
+        <v>1827.313601985166</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1827.313601985166</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1218.272576519721</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>55</v>
+        <v>152</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>L1MP</t>
+          <t>R U6RP</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1811.725144717046</v>
+        <v>0.2684678751731779</v>
       </c>
       <c r="D46" t="n">
-        <v>1811.725144717046</v>
+        <v>1047.890738579171</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1047.890738579171</v>
+      </c>
+      <c r="F46" t="n">
+        <v>698.6833150111717</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>56</v>
+        <v>153</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>R L1CP</t>
+          <t>L U6CP</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1811.725144717046</v>
+        <v>2232.613490956283</v>
       </c>
       <c r="D47" t="n">
-        <v>1811.725144717046</v>
+        <v>2528.794179050561</v>
+      </c>
+      <c r="E47" t="n">
+        <v>2528.794179050561</v>
+      </c>
+      <c r="F47" t="n">
+        <v>2430.067283019135</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>57</v>
+        <v>154</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>R L1RP</t>
+          <t>L U6RP</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1764.959772912686</v>
+        <v>2232.613490956283</v>
       </c>
       <c r="D48" t="n">
-        <v>1764.959772912686</v>
+        <v>782.8869650211325</v>
+      </c>
+      <c r="E48" t="n">
+        <v>782.8869650211325</v>
+      </c>
+      <c r="F48" t="n">
+        <v>1266.129140332849</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>58</v>
+        <v>155</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>L L1CP</t>
+          <t>L1MP</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1780.548230180806</v>
+        <v>1811.725144717046</v>
       </c>
       <c r="D49" t="n">
-        <v>1780.548230180806</v>
+        <v>2840.563324412959</v>
+      </c>
+      <c r="E49" t="n">
+        <v>2840.563324412959</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2497.617264514321</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>L L1RP</t>
+          <t>R L1CP</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1858.490516521405</v>
+        <v>1811.725144717046</v>
       </c>
       <c r="D50" t="n">
-        <v>1858.490516521405</v>
+        <v>1811.725144717046</v>
+      </c>
+      <c r="E50" t="n">
+        <v>1811.725144717046</v>
+      </c>
+      <c r="F50" t="n">
+        <v>1811.725144717046</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>R L3CP</t>
+          <t>R L1RP</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1827.313601985166</v>
+        <v>1764.959772912686</v>
       </c>
       <c r="D51" t="n">
-        <v>1827.313601985166</v>
+        <v>1796.136687448926</v>
+      </c>
+      <c r="E51" t="n">
+        <v>1796.136687448926</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1785.744382603513</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>R L3RP</t>
+          <t>L L1CP</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1593.486742963367</v>
+        <v>1780.548230180806</v>
       </c>
       <c r="D52" t="n">
-        <v>1593.486742963367</v>
+        <v>1796.136687448926</v>
+      </c>
+      <c r="E52" t="n">
+        <v>1796.136687448926</v>
+      </c>
+      <c r="F52" t="n">
+        <v>1790.940535026219</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>L L3CP</t>
+          <t>L L1RP</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1593.486742963367</v>
+        <v>1858.490516521405</v>
       </c>
       <c r="D53" t="n">
-        <v>1593.486742963367</v>
+        <v>1796.136687448926</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1796.136687448926</v>
+      </c>
+      <c r="F53" t="n">
+        <v>1816.921297139752</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>L L3RP</t>
+          <t>R L3CP</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>2029.963546470724</v>
+        <v>1827.313601985166</v>
       </c>
       <c r="D54" t="n">
-        <v>2029.963546470724</v>
+        <v>1.009785620812653</v>
+      </c>
+      <c r="E54" t="n">
+        <v>1.009785620812653</v>
+      </c>
+      <c r="F54" t="n">
+        <v>609.7777244089305</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>R L6CP</t>
+          <t>R L3RP</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1983.198174666365</v>
+        <v>1593.486742963367</v>
       </c>
       <c r="D55" t="n">
-        <v>1983.198174666365</v>
+        <v>2575.55955085492</v>
+      </c>
+      <c r="E55" t="n">
+        <v>2575.55955085492</v>
+      </c>
+      <c r="F55" t="n">
+        <v>2248.201948224403</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>R L6RP</t>
+          <t>L L3CP</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.7915472190589905</v>
+        <v>1593.486742963367</v>
       </c>
       <c r="D56" t="n">
-        <v>0.7915472190589905</v>
+        <v>0.02771281292108668</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.02771281292108668</v>
+      </c>
+      <c r="F56" t="n">
+        <v>531.1807228630697</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>L L6CP</t>
+          <t>L L3RP</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1.134493278957617</v>
+        <v>2029.963546470724</v>
       </c>
       <c r="D57" t="n">
-        <v>1.134493278957617</v>
+        <v>2591.148008123041</v>
+      </c>
+      <c r="E57" t="n">
+        <v>2591.148008123041</v>
+      </c>
+      <c r="F57" t="n">
+        <v>2404.086520905601</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>L L6RP</t>
+          <t>R L6CP</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>2123.494290079444</v>
+        <v>1983.198174666365</v>
       </c>
       <c r="D58" t="n">
-        <v>2123.494290079444</v>
+        <v>1.072139449885135</v>
+      </c>
+      <c r="E58" t="n">
+        <v>1.072139449885135</v>
+      </c>
+      <c r="F58" t="n">
+        <v>661.7808178553784</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Stomion super</t>
+          <t>R L6RP</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2185.848119151923</v>
+        <v>0.7915472190589905</v>
       </c>
       <c r="D59" t="n">
-        <v>2185.848119151923</v>
+        <v>2482.028807246201</v>
+      </c>
+      <c r="E59" t="n">
+        <v>2482.028807246201</v>
+      </c>
+      <c r="F59" t="n">
+        <v>1654.949720570487</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columella	</t>
+          <t>L L6CP</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1811.725144717046</v>
+        <v>1.134493278957617</v>
       </c>
       <c r="D60" t="n">
-        <v>1811.725144717046</v>
+        <v>0.635662646377761</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.635662646377761</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.8019395239043797</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Subnasale	</t>
+          <t>L L6RP</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1827.313601985166</v>
+        <v>2123.494290079444</v>
       </c>
       <c r="D61" t="n">
-        <v>1827.313601985166</v>
+        <v>2544.382636318681</v>
+      </c>
+      <c r="E61" t="n">
+        <v>2544.382636318681</v>
+      </c>
+      <c r="F61" t="n">
+        <v>2404.086520905602</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t xml:space="preserve">Upper lip	</t>
+          <t>Stomion super</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1842.902059253285</v>
+        <v>2185.848119151923</v>
       </c>
       <c r="D62" t="n">
-        <v>1842.902059253285</v>
+        <v>0.4018357873559784</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.4018357873559784</v>
+      </c>
+      <c r="F62" t="n">
+        <v>728.8839302422117</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>S Pogonion</t>
+          <t xml:space="preserve">Columella	</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1827.313601985166</v>
+        <v>1811.725144717046</v>
       </c>
       <c r="D63" t="n">
-        <v>1827.313601985166</v>
+        <v>2513.205721782441</v>
+      </c>
+      <c r="E63" t="n">
+        <v>2513.205721782441</v>
+      </c>
+      <c r="F63" t="n">
+        <v>2279.378862760643</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>R U2CP</t>
+          <t xml:space="preserve">Subnasale	</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1842.902059253285</v>
+        <v>1827.313601985166</v>
       </c>
       <c r="D64" t="n">
-        <v>1842.902059253285</v>
+        <v>1.087727907153255</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1.087727907153255</v>
+      </c>
+      <c r="F64" t="n">
+        <v>609.8296859331575</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>R U2RP</t>
+          <t xml:space="preserve">Upper lip	</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1640.252114767727</v>
+        <v>1842.902059253285</v>
       </c>
       <c r="D65" t="n">
-        <v>1640.252114767727</v>
+        <v>2497.617264514321</v>
+      </c>
+      <c r="E65" t="n">
+        <v>2497.617264514321</v>
+      </c>
+      <c r="F65" t="n">
+        <v>2279.378862760642</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>L U2CP</t>
+          <t>S Pogonion</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1671.429029303966</v>
+        <v>1827.313601985166</v>
       </c>
       <c r="D66" t="n">
-        <v>1671.429029303966</v>
+        <v>1905.255888325765</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1905.255888325765</v>
+      </c>
+      <c r="F66" t="n">
+        <v>1879.275126212232</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>L U2RP</t>
+          <t>R U2CP</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>2014.375089202604</v>
+        <v>1842.902059253285</v>
       </c>
       <c r="D67" t="n">
-        <v>2014.375089202604</v>
+        <v>1749.371315644566</v>
+      </c>
+      <c r="E67" t="n">
+        <v>1749.371315644566</v>
+      </c>
+      <c r="F67" t="n">
+        <v>1780.548230180805</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>R U4CP</t>
+          <t>R U2RP</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1952.021260130125</v>
+        <v>1640.252114767727</v>
       </c>
       <c r="D68" t="n">
-        <v>1952.021260130125</v>
+        <v>1827.313601985166</v>
+      </c>
+      <c r="E68" t="n">
+        <v>1827.313601985166</v>
+      </c>
+      <c r="F68" t="n">
+        <v>1764.959772912686</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>R U4RP</t>
+          <t>L U2CP</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1546721.371159007</v>
+        <v>1671.429029303966</v>
       </c>
       <c r="D69" t="n">
-        <v>1546721.371159007</v>
+        <v>1827.313601985166</v>
+      </c>
+      <c r="E69" t="n">
+        <v>1827.313601985166</v>
+      </c>
+      <c r="F69" t="n">
+        <v>1775.352077758099</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>L U4CP</t>
+          <t>L U2RP</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1546721.371159007</v>
+        <v>2014.375089202604</v>
       </c>
       <c r="D70" t="n">
-        <v>1546721.371159007</v>
+        <v>1764.959772912686</v>
+      </c>
+      <c r="E70" t="n">
+        <v>1764.959772912686</v>
+      </c>
+      <c r="F70" t="n">
+        <v>1848.098211675992</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>L U4RP</t>
+          <t>R U4CP</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1546721.371159007</v>
+        <v>1952.021260130125</v>
       </c>
       <c r="D71" t="n">
-        <v>1546721.371159007</v>
+        <v>1780.548230180806</v>
+      </c>
+      <c r="E71" t="n">
+        <v>1780.548230180806</v>
+      </c>
+      <c r="F71" t="n">
+        <v>1837.705906830579</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>R U5CP</t>
+          <t>R U4RP</t>
         </is>
       </c>
       <c r="C72" t="n">
         <v>1546721.371159007</v>
       </c>
       <c r="D72" t="n">
-        <v>1546721.371159007</v>
+        <v>0.9162548772039298</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.9162548772039298</v>
+      </c>
+      <c r="F72" t="n">
+        <v>515574.4012229205</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>R U5RP</t>
+          <t>L U4CP</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0.1212435565298096</v>
+        <v>1546721.371159007</v>
       </c>
       <c r="D73" t="n">
-        <v>0.1212435565298096</v>
+        <v>1577.898285695247</v>
+      </c>
+      <c r="E73" t="n">
+        <v>1577.898285695247</v>
+      </c>
+      <c r="F73" t="n">
+        <v>516625.7225767993</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>L U5CP</t>
+          <t>L U4RP</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.2528794179050575</v>
+        <v>1546721.371159007</v>
       </c>
       <c r="D74" t="n">
-        <v>0.2528794179050575</v>
+        <v>0.1905255888325755</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.1905255888325755</v>
+      </c>
+      <c r="F74" t="n">
+        <v>515573.9174033949</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>L U5RP</t>
+          <t>R U5CP</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>2185.848119151923</v>
+        <v>1546721.371159007</v>
       </c>
       <c r="D75" t="n">
-        <v>2185.848119151923</v>
+        <v>0.2684678751731779</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.2684678751731779</v>
+      </c>
+      <c r="F75" t="n">
+        <v>515573.9693649192</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>91</v>
+        <v>176</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>R U7CP</t>
+          <t>R U5RP</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>2154.671204615684</v>
+        <v>0.1212435565298096</v>
       </c>
       <c r="D76" t="n">
-        <v>2154.671204615684</v>
+        <v>1531.132913890887</v>
+      </c>
+      <c r="E76" t="n">
+        <v>1531.132913890887</v>
+      </c>
+      <c r="F76" t="n">
+        <v>1020.795690446102</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>R U7RP</t>
+          <t>L U5CP</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0.9630202490082912</v>
+        <v>0.2528794179050575</v>
       </c>
       <c r="D77" t="n">
-        <v>0.9630202490082912</v>
+        <v>1889.667431057645</v>
+      </c>
+      <c r="E77" t="n">
+        <v>1889.667431057645</v>
+      </c>
+      <c r="F77" t="n">
+        <v>1259.862580511065</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>L U7CP</t>
+          <t>L U5RP</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.2771281292110391</v>
+        <v>2185.848119151923</v>
       </c>
       <c r="D78" t="n">
-        <v>0.2771281292110391</v>
+        <v>1874.078973789525</v>
+      </c>
+      <c r="E78" t="n">
+        <v>1874.078973789525</v>
+      </c>
+      <c r="F78" t="n">
+        <v>1978.002022243658</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>L U7RP</t>
+          <t>R U7CP</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>2279.378862760643</v>
+        <v>2154.671204615684</v>
       </c>
       <c r="D79" t="n">
-        <v>2279.378862760643</v>
+        <v>2123.494290079444</v>
+      </c>
+      <c r="E79" t="n">
+        <v>2123.494290079444</v>
+      </c>
+      <c r="F79" t="n">
+        <v>2133.886594924857</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>R L2CP</t>
+          <t>R U7RP</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>2248.201948224403</v>
+        <v>0.9630202490082912</v>
       </c>
       <c r="D80" t="n">
-        <v>2248.201948224403</v>
+        <v>2061.140461006964</v>
+      </c>
+      <c r="E80" t="n">
+        <v>2061.140461006964</v>
+      </c>
+      <c r="F80" t="n">
+        <v>1374.414647420979</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>R L2RP</t>
+          <t>L U7CP</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>1687.017486572086</v>
+        <v>0.2771281292110391</v>
       </c>
       <c r="D81" t="n">
-        <v>1687.017486572086</v>
+        <v>2232.613490956283</v>
+      </c>
+      <c r="E81" t="n">
+        <v>2232.613490956283</v>
+      </c>
+      <c r="F81" t="n">
+        <v>1488.501370013925</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>L L2CP</t>
+          <t>L U7RP</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>1687.017486572086</v>
+        <v>2279.378862760643</v>
       </c>
       <c r="D82" t="n">
-        <v>1687.017486572086</v>
+        <v>2232.613490956283</v>
+      </c>
+      <c r="E82" t="n">
+        <v>2232.613490956283</v>
+      </c>
+      <c r="F82" t="n">
+        <v>2248.201948224403</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>98</v>
+        <v>180</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>L L2RP</t>
+          <t>R L2CP</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1936.432802862005</v>
+        <v>2248.201948224403</v>
       </c>
       <c r="D83" t="n">
-        <v>1936.432802862005</v>
+        <v>2061.140461006964</v>
+      </c>
+      <c r="E83" t="n">
+        <v>2061.140461006964</v>
+      </c>
+      <c r="F83" t="n">
+        <v>2123.494290079444</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>R L4CP</t>
+          <t>R L2RP</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>1905.255888325765</v>
+        <v>1687.017486572086</v>
       </c>
       <c r="D84" t="n">
-        <v>1905.255888325765</v>
+        <v>1811.725144717046</v>
+      </c>
+      <c r="E84" t="n">
+        <v>1811.725144717046</v>
+      </c>
+      <c r="F84" t="n">
+        <v>1770.155925335393</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>R L4RP</t>
+          <t>L L2CP</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>1499.955999354648</v>
+        <v>1687.017486572086</v>
       </c>
       <c r="D85" t="n">
-        <v>1499.955999354648</v>
+        <v>1811.725144717046</v>
+      </c>
+      <c r="E85" t="n">
+        <v>1811.725144717046</v>
+      </c>
+      <c r="F85" t="n">
+        <v>1770.155925335393</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>L L4CP</t>
+          <t>L L2RP</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1531.132913890887</v>
+        <v>1936.432802862005</v>
       </c>
       <c r="D86" t="n">
-        <v>1531.132913890887</v>
+        <v>1764.959772912686</v>
+      </c>
+      <c r="E86" t="n">
+        <v>1764.959772912686</v>
+      </c>
+      <c r="F86" t="n">
+        <v>1822.117449562459</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>L L4RP</t>
+          <t>R L4CP</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>2061.140461006964</v>
+        <v>1905.255888325765</v>
       </c>
       <c r="D87" t="n">
-        <v>2061.140461006964</v>
+        <v>1780.548230180806</v>
+      </c>
+      <c r="E87" t="n">
+        <v>1780.548230180806</v>
+      </c>
+      <c r="F87" t="n">
+        <v>1822.117449562459</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>R L5CP</t>
+          <t>R L4RP</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>2061.140461006964</v>
+        <v>1499.955999354648</v>
       </c>
       <c r="D88" t="n">
-        <v>2061.140461006964</v>
+        <v>1593.486742963367</v>
+      </c>
+      <c r="E88" t="n">
+        <v>1593.486742963367</v>
+      </c>
+      <c r="F88" t="n">
+        <v>1562.309828427127</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>R L5RP</t>
+          <t>L L4CP</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1437602.170282168</v>
+        <v>1531.132913890887</v>
       </c>
       <c r="D89" t="n">
-        <v>1437602.170282168</v>
+        <v>1593.486742963367</v>
+      </c>
+      <c r="E89" t="n">
+        <v>1593.486742963367</v>
+      </c>
+      <c r="F89" t="n">
+        <v>1572.702133272541</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>L L5CP</t>
+          <t>L L4RP</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>1437602.170282168</v>
+        <v>2061.140461006964</v>
       </c>
       <c r="D90" t="n">
-        <v>1437602.170282168</v>
+        <v>0.7915472190589905</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.7915472190589905</v>
+      </c>
+      <c r="F90" t="n">
+        <v>687.5745184816939</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>L L5RP</t>
+          <t>R L5CP</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>1437602.170282168</v>
+        <v>2061.140461006964</v>
       </c>
       <c r="D91" t="n">
-        <v>1437602.170282168</v>
+        <v>1.134493278957617</v>
+      </c>
+      <c r="E91" t="n">
+        <v>1.134493278957617</v>
+      </c>
+      <c r="F91" t="n">
+        <v>687.803149188293</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>R L7CP</t>
+          <t>R L5RP</t>
         </is>
       </c>
       <c r="C92" t="n">
         <v>1437602.170282168</v>
       </c>
       <c r="D92" t="n">
-        <v>1437602.170282168</v>
+        <v>1858.490516521405</v>
+      </c>
+      <c r="E92" t="n">
+        <v>1858.490516521405</v>
+      </c>
+      <c r="F92" t="n">
+        <v>480439.7171050704</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>R L7RP</t>
+          <t>L L5CP</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1390.836798477809</v>
+        <v>1437602.170282168</v>
       </c>
       <c r="D93" t="n">
-        <v>1390.836798477809</v>
+        <v>1827.313601985166</v>
+      </c>
+      <c r="E93" t="n">
+        <v>1827.313601985166</v>
+      </c>
+      <c r="F93" t="n">
+        <v>480418.9324953794</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>109</v>
+        <v>63</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>L L7CP</t>
+          <t>L L5RP</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1406.425255745928</v>
+        <v>1437602.170282168</v>
       </c>
       <c r="D94" t="n">
-        <v>1406.425255745928</v>
+        <v>2029.963546470724</v>
+      </c>
+      <c r="E94" t="n">
+        <v>2029.963546470724</v>
+      </c>
+      <c r="F94" t="n">
+        <v>480554.0324583699</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>110</v>
+        <v>64</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>L L7RP</t>
+          <t>R L7CP</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>2217.025033688163</v>
+        <v>1437602.170282168</v>
       </c>
       <c r="D95" t="n">
-        <v>2217.025033688163</v>
+        <v>1983.198174666365</v>
+      </c>
+      <c r="E95" t="n">
+        <v>1983.198174666365</v>
+      </c>
+      <c r="F95" t="n">
+        <v>480522.8555438336</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>R U8CP</t>
+          <t>R L7RP</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>2217.025033688163</v>
+        <v>1390.836798477809</v>
       </c>
       <c r="D96" t="n">
-        <v>2217.025033688163</v>
+        <v>2123.494290079444</v>
+      </c>
+      <c r="E96" t="n">
+        <v>2123.494290079444</v>
+      </c>
+      <c r="F96" t="n">
+        <v>1879.275126212232</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>R U8RP</t>
+          <t>L L7CP</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1312.894512137209</v>
+        <v>1406.425255745928</v>
       </c>
       <c r="D97" t="n">
-        <v>1312.894512137209</v>
+        <v>2185.848119151923</v>
+      </c>
+      <c r="E97" t="n">
+        <v>2185.848119151923</v>
+      </c>
+      <c r="F97" t="n">
+        <v>1926.040498016591</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>L U8CP</t>
+          <t>L L7RP</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>1359.659883941569</v>
+        <v>2217.025033688163</v>
       </c>
       <c r="D98" t="n">
-        <v>1359.659883941569</v>
+        <v>1811.725144717046</v>
+      </c>
+      <c r="E98" t="n">
+        <v>1811.725144717046</v>
+      </c>
+      <c r="F98" t="n">
+        <v>1946.825107707418</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>L U8RP</t>
+          <t>R U8CP</t>
         </is>
       </c>
       <c r="C99" t="n">
         <v>2217.025033688163</v>
       </c>
       <c r="D99" t="n">
-        <v>2217.025033688163</v>
+        <v>1640.252114767727</v>
+      </c>
+      <c r="E99" t="n">
+        <v>1640.252114767727</v>
+      </c>
+      <c r="F99" t="n">
+        <v>1832.509754407872</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>R L8CP</t>
+          <t>R U8RP</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>2217.025033688163</v>
+        <v>1312.894512137209</v>
       </c>
       <c r="D100" t="n">
-        <v>2217.025033688163</v>
+        <v>1671.429029303966</v>
+      </c>
+      <c r="E100" t="n">
+        <v>1671.429029303966</v>
+      </c>
+      <c r="F100" t="n">
+        <v>1551.917523581714</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>R L8RP</t>
+          <t>L U8CP</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>1297.306054869089</v>
+        <v>1359.659883941569</v>
       </c>
       <c r="D101" t="n">
-        <v>1297.306054869089</v>
+        <v>1546721.371159007</v>
+      </c>
+      <c r="E101" t="n">
+        <v>1546721.371159007</v>
+      </c>
+      <c r="F101" t="n">
+        <v>1031600.800733985</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>L L8CP</t>
+          <t>L U8RP</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>1188.18685399225</v>
+        <v>2217.025033688163</v>
       </c>
       <c r="D102" t="n">
-        <v>1188.18685399225</v>
+        <v>1546721.371159007</v>
+      </c>
+      <c r="E102" t="n">
+        <v>1546721.371159007</v>
+      </c>
+      <c r="F102" t="n">
+        <v>1031886.589117234</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>118</v>
+        <v>174</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>L L8RP</t>
+          <t>R L8CP</t>
         </is>
       </c>
       <c r="C103" t="n">
         <v>2217.025033688163</v>
       </c>
       <c r="D103" t="n">
-        <v>2217.025033688163</v>
+        <v>1437602.170282168</v>
+      </c>
+      <c r="E103" t="n">
+        <v>1437602.170282168</v>
+      </c>
+      <c r="F103" t="n">
+        <v>959140.4551993414</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>S Glabella</t>
+          <t>R L8RP</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2372.909606369362</v>
+        <v>1297.306054869089</v>
       </c>
       <c r="D104" t="n">
-        <v>2372.909606369362</v>
+        <v>0.1212435565298096</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0.1212435565298096</v>
+      </c>
+      <c r="F104" t="n">
+        <v>432.5161806607162</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>S Nasion</t>
+          <t>L L8CP</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>1749.371315644566</v>
+        <v>1188.18685399225</v>
       </c>
       <c r="D105" t="n">
-        <v>1749.371315644566</v>
+        <v>0.2528794179050575</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0.2528794179050575</v>
+      </c>
+      <c r="F105" t="n">
+        <v>396.2308709426866</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>121</v>
+        <v>175</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Pronasale</t>
+          <t>L L8RP</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1749.371315644566</v>
+        <v>2217.025033688163</v>
       </c>
       <c r="D106" t="n">
-        <v>1749.371315644566</v>
+        <v>1484.367542086528</v>
+      </c>
+      <c r="E106" t="n">
+        <v>1484.367542086528</v>
+      </c>
+      <c r="F106" t="n">
+        <v>1728.58670595374</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Lower lip</t>
+          <t>S Glabella</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>1749.371315644566</v>
+        <v>2372.909606369362</v>
       </c>
       <c r="D107" t="n">
-        <v>1749.371315644566</v>
+        <v>0.9630202490082912</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0.9630202490082912</v>
+      </c>
+      <c r="F107" t="n">
+        <v>791.6118822891262</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Mentolabial Sulc</t>
+          <t>S Nasion</t>
         </is>
       </c>
       <c r="C108" t="n">
         <v>1749.371315644566</v>
       </c>
       <c r="D108" t="n">
-        <v>1749.371315644566</v>
+        <v>0.2771281292110391</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0.2771281292110391</v>
+      </c>
+      <c r="F108" t="n">
+        <v>583.3085239676626</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>125</v>
+        <v>177</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Base of Epiglott</t>
+          <t>Pronasale</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>969.9484522385712</v>
+        <v>1749.371315644566</v>
       </c>
       <c r="D109" t="n">
-        <v>969.9484522385712</v>
+        <v>1484.367542086528</v>
+      </c>
+      <c r="E109" t="n">
+        <v>1484.367542086528</v>
+      </c>
+      <c r="F109" t="n">
+        <v>1572.702133272541</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>R Cd-L</t>
+          <t>Lower lip</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>1905.255888325765</v>
+        <v>1749.371315644566</v>
       </c>
       <c r="D110" t="n">
-        <v>1905.255888325765</v>
+        <v>1312.894512137209</v>
+      </c>
+      <c r="E110" t="n">
+        <v>1312.894512137209</v>
+      </c>
+      <c r="F110" t="n">
+        <v>1458.386779972995</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>R Cd-M</t>
+          <t>Mentolabial Sulc</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>829.6523368254922</v>
+        <v>1749.371315644566</v>
       </c>
       <c r="D111" t="n">
-        <v>829.6523368254922</v>
+        <v>1359.659883941569</v>
+      </c>
+      <c r="E111" t="n">
+        <v>1359.659883941569</v>
+      </c>
+      <c r="F111" t="n">
+        <v>1489.563694509234</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>R C Cd-S</t>
+          <t>Base of Epiglott</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>1110.24456765165</v>
+        <v>969.9484522385712</v>
       </c>
       <c r="D112" t="n">
-        <v>1110.24456765165</v>
+        <v>2014.375089202604</v>
+      </c>
+      <c r="E112" t="n">
+        <v>2014.375089202604</v>
+      </c>
+      <c r="F112" t="n">
+        <v>1666.23287688126</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>129</v>
+        <v>83</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>R GF-L</t>
+          <t>R Cd-L</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>969.9484522385712</v>
+        <v>1905.255888325765</v>
       </c>
       <c r="D113" t="n">
-        <v>969.9484522385712</v>
+        <v>1952.021260130125</v>
+      </c>
+      <c r="E113" t="n">
+        <v>1952.021260130125</v>
+      </c>
+      <c r="F113" t="n">
+        <v>1936.432802862005</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>R GF-M</t>
+          <t>R Cd-M</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>814.0638795573723</v>
+        <v>829.6523368254922</v>
       </c>
       <c r="D114" t="n">
-        <v>814.0638795573723</v>
+        <v>1546721.371159007</v>
+      </c>
+      <c r="E114" t="n">
+        <v>1546721.371159007</v>
+      </c>
+      <c r="F114" t="n">
+        <v>1031424.131551613</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>R C GF-S</t>
+          <t>R C Cd-S</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>1188.18685399225</v>
+        <v>1110.24456765165</v>
       </c>
       <c r="D115" t="n">
-        <v>1188.18685399225</v>
+        <v>1546721.371159007</v>
+      </c>
+      <c r="E115" t="n">
+        <v>1546721.371159007</v>
+      </c>
+      <c r="F115" t="n">
+        <v>1031517.662295222</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>132</v>
+        <v>178</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>R Cd-A</t>
+          <t>R GF-L</t>
         </is>
       </c>
       <c r="C116" t="n">
         <v>969.9484522385712</v>
       </c>
       <c r="D116" t="n">
-        <v>969.9484522385712</v>
+        <v>1437602.170282168</v>
+      </c>
+      <c r="E116" t="n">
+        <v>1437602.170282168</v>
+      </c>
+      <c r="F116" t="n">
+        <v>958724.7630055249</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>133</v>
+        <v>90</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>R Cd-P</t>
+          <t>R GF-M</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>985.5369095066911</v>
+        <v>814.0638795573723</v>
       </c>
       <c r="D117" t="n">
-        <v>985.5369095066911</v>
+        <v>2185.848119151923</v>
+      </c>
+      <c r="E117" t="n">
+        <v>2185.848119151923</v>
+      </c>
+      <c r="F117" t="n">
+        <v>1728.58670595374</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>R S Cd-S</t>
+          <t>R C GF-S</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>923.1830804342115</v>
+        <v>1188.18685399225</v>
       </c>
       <c r="D118" t="n">
-        <v>923.1830804342115</v>
+        <v>2154.671204615684</v>
+      </c>
+      <c r="E118" t="n">
+        <v>2154.671204615684</v>
+      </c>
+      <c r="F118" t="n">
+        <v>1832.509754407873</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>135</v>
+        <v>179</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>R GF-A</t>
+          <t>R Cd-A</t>
         </is>
       </c>
       <c r="C119" t="n">
         <v>969.9484522385712</v>
       </c>
       <c r="D119" t="n">
-        <v>969.9484522385712</v>
+        <v>2061.140461006964</v>
+      </c>
+      <c r="E119" t="n">
+        <v>2061.140461006964</v>
+      </c>
+      <c r="F119" t="n">
+        <v>1697.4097914175</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>136</v>
+        <v>94</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>R GF-P</t>
+          <t>R Cd-P</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>1001.125366774811</v>
+        <v>985.5369095066911</v>
       </c>
       <c r="D120" t="n">
-        <v>1001.125366774811</v>
+        <v>2279.378862760643</v>
+      </c>
+      <c r="E120" t="n">
+        <v>2279.378862760643</v>
+      </c>
+      <c r="F120" t="n">
+        <v>1848.098211675992</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>137</v>
+        <v>95</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>R S GF-S</t>
+          <t>R S Cd-S</t>
         </is>
       </c>
       <c r="C121" t="n">
         <v>923.1830804342115</v>
       </c>
       <c r="D121" t="n">
-        <v>923.1830804342115</v>
+        <v>2248.201948224403</v>
+      </c>
+      <c r="E121" t="n">
+        <v>2248.201948224403</v>
+      </c>
+      <c r="F121" t="n">
+        <v>1806.528992294339</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>138</v>
+        <v>181</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>L Cd-L</t>
+          <t>R GF-A</t>
         </is>
       </c>
       <c r="C122" t="n">
         <v>969.9484522385712</v>
       </c>
       <c r="D122" t="n">
-        <v>969.9484522385712</v>
+        <v>2061.140461006964</v>
+      </c>
+      <c r="E122" t="n">
+        <v>2061.140461006964</v>
+      </c>
+      <c r="F122" t="n">
+        <v>1697.4097914175</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>L Cd-M</t>
+          <t>R GF-P</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>2684.67875173176</v>
+        <v>1001.125366774811</v>
       </c>
       <c r="D123" t="n">
-        <v>2684.67875173176</v>
+        <v>2217.025033688163</v>
+      </c>
+      <c r="E123" t="n">
+        <v>2217.025033688163</v>
+      </c>
+      <c r="F123" t="n">
+        <v>1811.725144717046</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>L C Cd-S</t>
+          <t>R S GF-S</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>2684.67875173176</v>
+        <v>923.1830804342115</v>
       </c>
       <c r="D124" t="n">
-        <v>2684.67875173176</v>
+        <v>2217.025033688163</v>
+      </c>
+      <c r="E124" t="n">
+        <v>2217.025033688163</v>
+      </c>
+      <c r="F124" t="n">
+        <v>1785.744382603513</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>L GF-L</t>
+          <t>L Cd-L</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>2528.794179050561</v>
+        <v>969.9484522385712</v>
       </c>
       <c r="D125" t="n">
-        <v>2528.794179050561</v>
+        <v>1687.017486572086</v>
+      </c>
+      <c r="E125" t="n">
+        <v>1687.017486572086</v>
+      </c>
+      <c r="F125" t="n">
+        <v>1447.994475127581</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>142</v>
+        <v>97</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>L GF-M</t>
+          <t>L Cd-M</t>
         </is>
       </c>
       <c r="C126" t="n">
         <v>2684.67875173176</v>
       </c>
       <c r="D126" t="n">
-        <v>2684.67875173176</v>
+        <v>1687.017486572086</v>
+      </c>
+      <c r="E126" t="n">
+        <v>1687.017486572086</v>
+      </c>
+      <c r="F126" t="n">
+        <v>2019.571241625311</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>L C GF-S</t>
+          <t>L C Cd-S</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>2840.563324412959</v>
+        <v>2684.67875173176</v>
       </c>
       <c r="D127" t="n">
-        <v>2840.563324412959</v>
+        <v>1499.955999354648</v>
+      </c>
+      <c r="E127" t="n">
+        <v>1499.955999354648</v>
+      </c>
+      <c r="F127" t="n">
+        <v>1894.863583480352</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>L Cd-A</t>
+          <t>L GF-L</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>2372.909606369362</v>
+        <v>2528.794179050561</v>
       </c>
       <c r="D128" t="n">
-        <v>2372.909606369362</v>
+        <v>1531.132913890887</v>
+      </c>
+      <c r="E128" t="n">
+        <v>1531.132913890887</v>
+      </c>
+      <c r="F128" t="n">
+        <v>1863.686668944112</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>145</v>
+        <v>104</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>L Cd-P</t>
+          <t>L GF-M</t>
         </is>
       </c>
       <c r="C129" t="n">
         <v>2684.67875173176</v>
       </c>
       <c r="D129" t="n">
-        <v>2684.67875173176</v>
+        <v>1437602.170282168</v>
+      </c>
+      <c r="E129" t="n">
+        <v>1437602.170282168</v>
+      </c>
+      <c r="F129" t="n">
+        <v>959296.3397720227</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>146</v>
+        <v>105</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>L S Cd-S</t>
+          <t>L C GF-S</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>2684.67875173176</v>
+        <v>2840.563324412959</v>
       </c>
       <c r="D130" t="n">
-        <v>2684.67875173176</v>
+        <v>1437602.170282168</v>
+      </c>
+      <c r="E130" t="n">
+        <v>1437602.170282168</v>
+      </c>
+      <c r="F130" t="n">
+        <v>959348.3012962496</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>147</v>
+        <v>108</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>L GF-A</t>
+          <t>L Cd-A</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>2684.67875173176</v>
+        <v>2372.909606369362</v>
       </c>
       <c r="D131" t="n">
-        <v>2684.67875173176</v>
+        <v>1390.836798477809</v>
+      </c>
+      <c r="E131" t="n">
+        <v>1390.836798477809</v>
+      </c>
+      <c r="F131" t="n">
+        <v>1718.194401108327</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>148</v>
+        <v>109</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>L GF-P</t>
+          <t>L Cd-P</t>
         </is>
       </c>
       <c r="C132" t="n">
         <v>2684.67875173176</v>
       </c>
       <c r="D132" t="n">
-        <v>2684.67875173176</v>
+        <v>1406.425255745928</v>
+      </c>
+      <c r="E132" t="n">
+        <v>1406.425255745928</v>
+      </c>
+      <c r="F132" t="n">
+        <v>1832.509754407872</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>L S GF-S</t>
+          <t>L S Cd-S</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>2528.794179050561</v>
+        <v>2684.67875173176</v>
       </c>
       <c r="D133" t="n">
-        <v>2528.794179050561</v>
+        <v>1297.306054869089</v>
+      </c>
+      <c r="E133" t="n">
+        <v>1297.306054869089</v>
+      </c>
+      <c r="F133" t="n">
+        <v>1759.763620489979</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>R Ant. Zygoma</t>
+          <t>L GF-A</t>
         </is>
       </c>
       <c r="C134" t="n">
         <v>2684.67875173176</v>
       </c>
       <c r="D134" t="n">
-        <v>2684.67875173176</v>
+        <v>1188.18685399225</v>
+      </c>
+      <c r="E134" t="n">
+        <v>1188.18685399225</v>
+      </c>
+      <c r="F134" t="n">
+        <v>1687.017486572086</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>151</v>
+        <v>98</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>L Ant. Zygoma</t>
+          <t>L GF-P</t>
         </is>
       </c>
       <c r="C135" t="n">
         <v>2684.67875173176</v>
       </c>
       <c r="D135" t="n">
-        <v>2684.67875173176</v>
+        <v>1936.432802862005</v>
+      </c>
+      <c r="E135" t="n">
+        <v>1936.432802862005</v>
+      </c>
+      <c r="F135" t="n">
+        <v>2185.848119151923</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>152</v>
+        <v>99</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>R Zygion</t>
+          <t>L S GF-S</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>1047.890738579171</v>
+        <v>2528.794179050561</v>
       </c>
       <c r="D136" t="n">
-        <v>1047.890738579171</v>
+        <v>1905.255888325765</v>
+      </c>
+      <c r="E136" t="n">
+        <v>1905.255888325765</v>
+      </c>
+      <c r="F136" t="n">
+        <v>2113.101985234031</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>153</v>
+        <v>102</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>L Zygion</t>
+          <t>R Ant. Zygoma</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2528.794179050561</v>
+        <v>2684.67875173176</v>
       </c>
       <c r="D137" t="n">
-        <v>2528.794179050561</v>
+        <v>2061.140461006964</v>
+      </c>
+      <c r="E137" t="n">
+        <v>2061.140461006964</v>
+      </c>
+      <c r="F137" t="n">
+        <v>2268.986557915229</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>154</v>
+        <v>103</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>R Endocanthion</t>
+          <t>L Ant. Zygoma</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>782.8869650211325</v>
+        <v>2684.67875173176</v>
       </c>
       <c r="D138" t="n">
-        <v>782.8869650211325</v>
+        <v>2061.140461006964</v>
+      </c>
+      <c r="E138" t="n">
+        <v>2061.140461006964</v>
+      </c>
+      <c r="F138" t="n">
+        <v>2268.986557915229</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>L Endocanthion</t>
+          <t>R Zygion</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>2840.563324412959</v>
+        <v>1047.890738579171</v>
       </c>
       <c r="D139" t="n">
-        <v>2840.563324412959</v>
+        <v>1437602.170282168</v>
+      </c>
+      <c r="E139" t="n">
+        <v>1437602.170282168</v>
+      </c>
+      <c r="F139" t="n">
+        <v>958750.7437676383</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>R Exocanthion</t>
+          <t>L Zygion</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>1531.132913890887</v>
+        <v>2528.794179050561</v>
       </c>
       <c r="D140" t="n">
-        <v>1531.132913890887</v>
+        <v>1437602.170282168</v>
+      </c>
+      <c r="E140" t="n">
+        <v>1437602.170282168</v>
+      </c>
+      <c r="F140" t="n">
+        <v>959244.3782477956</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>157</v>
+        <v>110</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>L Exocanthion</t>
+          <t>R Endocanthion</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>2061.140461006964</v>
+        <v>782.8869650211325</v>
       </c>
       <c r="D141" t="n">
-        <v>2061.140461006964</v>
+        <v>2217.025033688163</v>
+      </c>
+      <c r="E141" t="n">
+        <v>2217.025033688163</v>
+      </c>
+      <c r="F141" t="n">
+        <v>1738.979010799153</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>158</v>
+        <v>111</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>R S Ant. Zygoma</t>
+          <t>L Endocanthion</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>1032.302281311051</v>
+        <v>2840.563324412959</v>
       </c>
       <c r="D142" t="n">
-        <v>1032.302281311051</v>
+        <v>2217.025033688163</v>
+      </c>
+      <c r="E142" t="n">
+        <v>2217.025033688163</v>
+      </c>
+      <c r="F142" t="n">
+        <v>2424.871130596428</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>159</v>
+        <v>118</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>L S Ant. Zygoma</t>
+          <t>R Exocanthion</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>2528.794179050561</v>
+        <v>1531.132913890887</v>
       </c>
       <c r="D143" t="n">
-        <v>2528.794179050561</v>
+        <v>2217.025033688163</v>
+      </c>
+      <c r="E143" t="n">
+        <v>2217.025033688163</v>
+      </c>
+      <c r="F143" t="n">
+        <v>1988.394327089071</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>R S Zygion</t>
+          <t>L Exocanthion</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>798.4754222892524</v>
+        <v>2061.140461006964</v>
       </c>
       <c r="D144" t="n">
-        <v>798.4754222892524</v>
+        <v>2372.909606369362</v>
+      </c>
+      <c r="E144" t="n">
+        <v>2372.909606369362</v>
+      </c>
+      <c r="F144" t="n">
+        <v>2268.986557915229</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>161</v>
+        <v>120</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>L S Zygion</t>
+          <t>R S Ant. Zygoma</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>2840.563324412959</v>
+        <v>1032.302281311051</v>
       </c>
       <c r="D145" t="n">
-        <v>2840.563324412959</v>
+        <v>1749.371315644566</v>
+      </c>
+      <c r="E145" t="n">
+        <v>1749.371315644566</v>
+      </c>
+      <c r="F145" t="n">
+        <v>1510.348304200061</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>162</v>
+        <v>121</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>R Alar</t>
+          <t>L S Ant. Zygoma</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>642.5908496080535</v>
+        <v>2528.794179050561</v>
       </c>
       <c r="D146" t="n">
-        <v>642.5908496080535</v>
+        <v>1749.371315644566</v>
+      </c>
+      <c r="E146" t="n">
+        <v>1749.371315644566</v>
+      </c>
+      <c r="F146" t="n">
+        <v>2009.178936779898</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>L Alar</t>
+          <t>R S Zygion</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>2996.447897094158</v>
+        <v>798.4754222892524</v>
       </c>
       <c r="D147" t="n">
-        <v>2996.447897094158</v>
+        <v>1531.132913890887</v>
+      </c>
+      <c r="E147" t="n">
+        <v>1531.132913890887</v>
+      </c>
+      <c r="F147" t="n">
+        <v>1286.913750023676</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Labiale Superius</t>
+          <t>L S Zygion</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>1546.721371159008</v>
+        <v>2840.563324412959</v>
       </c>
       <c r="D148" t="n">
-        <v>1546.721371159008</v>
+        <v>2061.140461006964</v>
+      </c>
+      <c r="E148" t="n">
+        <v>2061.140461006964</v>
+      </c>
+      <c r="F148" t="n">
+        <v>2320.948082142295</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>R Crista Philtri</t>
+          <t>R Alar</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>2061.140461006964</v>
+        <v>642.5908496080535</v>
       </c>
       <c r="D149" t="n">
-        <v>2061.140461006964</v>
+        <v>1032.302281311051</v>
+      </c>
+      <c r="E149" t="n">
+        <v>1032.302281311051</v>
+      </c>
+      <c r="F149" t="n">
+        <v>902.3984707433851</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>L Crista Philtri</t>
+          <t>L Alar</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>1749.371315644566</v>
+        <v>2996.447897094158</v>
       </c>
       <c r="D150" t="n">
-        <v>1749.371315644566</v>
+        <v>2528.794179050561</v>
+      </c>
+      <c r="E150" t="n">
+        <v>2528.794179050561</v>
+      </c>
+      <c r="F150" t="n">
+        <v>2684.67875173176</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>R Cheilion</t>
+          <t>Labiale Superius</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>1749.371315644566</v>
+        <v>1546.721371159008</v>
       </c>
       <c r="D151" t="n">
-        <v>1749.371315644566</v>
+        <v>798.4754222892524</v>
+      </c>
+      <c r="E151" t="n">
+        <v>798.4754222892524</v>
+      </c>
+      <c r="F151" t="n">
+        <v>1047.890738579171</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>L Cheilion</t>
+          <t>R Crista Philtri</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>1905.255888325765</v>
+        <v>2061.140461006964</v>
       </c>
       <c r="D152" t="n">
-        <v>1905.255888325765</v>
+        <v>2840.563324412959</v>
+      </c>
+      <c r="E152" t="n">
+        <v>2840.563324412959</v>
+      </c>
+      <c r="F152" t="n">
+        <v>2580.755703277627</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Labiale Inferius</t>
+          <t>L Crista Philtri</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>1468.779084818408</v>
+        <v>1749.371315644566</v>
       </c>
       <c r="D153" t="n">
-        <v>1468.779084818408</v>
+        <v>642.5908496080535</v>
+      </c>
+      <c r="E153" t="n">
+        <v>642.5908496080535</v>
+      </c>
+      <c r="F153" t="n">
+        <v>1011.517671620224</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>R S Go</t>
+          <t>R Cheilion</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>2061.140461006964</v>
+        <v>1749.371315644566</v>
       </c>
       <c r="D154" t="n">
-        <v>2061.140461006964</v>
+        <v>2996.447897094158</v>
+      </c>
+      <c r="E154" t="n">
+        <v>2996.447897094158</v>
+      </c>
+      <c r="F154" t="n">
+        <v>2580.755703277628</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>L S Go</t>
+          <t>L Cheilion</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>1749.371315644566</v>
+        <v>1905.255888325765</v>
       </c>
       <c r="D155" t="n">
-        <v>1749.371315644566</v>
+        <v>1546.721371159008</v>
+      </c>
+      <c r="E155" t="n">
+        <v>1546.721371159008</v>
+      </c>
+      <c r="F155" t="n">
+        <v>1666.23287688126</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>R U4PRP</t>
+          <t>Labiale Inferius</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>1437602.170282168</v>
+        <v>1468.779084818408</v>
       </c>
       <c r="D156" t="n">
-        <v>1437602.170282168</v>
+        <v>2061.140461006964</v>
+      </c>
+      <c r="E156" t="n">
+        <v>2061.140461006964</v>
+      </c>
+      <c r="F156" t="n">
+        <v>1863.686668944112</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>175</v>
+        <v>71</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>R U5PRP</t>
+          <t>R S Go</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>1484.367542086528</v>
+        <v>2061.140461006964</v>
       </c>
       <c r="D157" t="n">
-        <v>1484.367542086528</v>
+        <v>1842.902059253285</v>
+      </c>
+      <c r="E157" t="n">
+        <v>1842.902059253285</v>
+      </c>
+      <c r="F157" t="n">
+        <v>1915.648193171178</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>176</v>
+        <v>72</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>R U6PRP</t>
+          <t>L S Go</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>1531.132913890887</v>
+        <v>1749.371315644566</v>
       </c>
       <c r="D158" t="n">
-        <v>1531.132913890887</v>
+        <v>1827.313601985166</v>
+      </c>
+      <c r="E158" t="n">
+        <v>1827.313601985166</v>
+      </c>
+      <c r="F158" t="n">
+        <v>1801.332839871632</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>R U7PRP</t>
+          <t>R U4PRP</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>1484.367542086528</v>
+        <v>1437602.170282168</v>
       </c>
       <c r="D159" t="n">
-        <v>1484.367542086528</v>
+        <v>1749.371315644566</v>
+      </c>
+      <c r="E159" t="n">
+        <v>1749.371315644566</v>
+      </c>
+      <c r="F159" t="n">
+        <v>480366.9709711524</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>L U4PRP</t>
+          <t>R U5PRP</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>1437602.170282168</v>
+        <v>1484.367542086528</v>
       </c>
       <c r="D160" t="n">
-        <v>1437602.170282168</v>
+        <v>1749.371315644566</v>
+      </c>
+      <c r="E160" t="n">
+        <v>1749.371315644566</v>
+      </c>
+      <c r="F160" t="n">
+        <v>1661.036724458553</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>L U5PRP</t>
+          <t>R U6PRP</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>2061.140461006964</v>
+        <v>1531.132913890887</v>
       </c>
       <c r="D161" t="n">
-        <v>2061.140461006964</v>
+        <v>1905.255888325765</v>
+      </c>
+      <c r="E161" t="n">
+        <v>1905.255888325765</v>
+      </c>
+      <c r="F161" t="n">
+        <v>1780.548230180806</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>180</v>
+        <v>73</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>L U6PRP</t>
+          <t>R U7PRP</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>2061.140461006964</v>
+        <v>1484.367542086528</v>
       </c>
       <c r="D162" t="n">
-        <v>2061.140461006964</v>
+        <v>1842.902059253285</v>
+      </c>
+      <c r="E162" t="n">
+        <v>1842.902059253285</v>
+      </c>
+      <c r="F162" t="n">
+        <v>1723.390553531033</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
+          <t>L U4PRP</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>1437602.170282168</v>
+      </c>
+      <c r="D163" t="n">
+        <v>1468.779084818408</v>
+      </c>
+      <c r="E163" t="n">
+        <v>1468.779084818408</v>
+      </c>
+      <c r="F163" t="n">
+        <v>480179.909483935</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>170</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>L U5PRP</t>
+        </is>
+      </c>
+      <c r="C164" t="n">
+        <v>2061.140461006964</v>
+      </c>
+      <c r="D164" t="n">
+        <v>2061.140461006964</v>
+      </c>
+      <c r="E164" t="n">
+        <v>2061.140461006964</v>
+      </c>
+      <c r="F164" t="n">
+        <v>2061.140461006964</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>123</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>L U6PRP</t>
+        </is>
+      </c>
+      <c r="C165" t="n">
+        <v>2061.140461006964</v>
+      </c>
+      <c r="D165" t="n">
+        <v>1749.371315644566</v>
+      </c>
+      <c r="E165" t="n">
+        <v>1749.371315644566</v>
+      </c>
+      <c r="F165" t="n">
+        <v>1853.294364098699</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>171</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
           <t>L U7PRP</t>
         </is>
       </c>
-      <c r="C163" t="n">
+      <c r="C166" t="n">
         <v>2061.140461006964</v>
       </c>
-      <c r="D163" t="n">
-        <v>2061.140461006964</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr"/>
-      <c r="B164" t="inlineStr">
+      <c r="D166" t="n">
+        <v>1749.371315644566</v>
+      </c>
+      <c r="E166" t="n">
+        <v>1749.371315644566</v>
+      </c>
+      <c r="F166" t="n">
+        <v>1853.294364098699</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="B167" t="inlineStr">
         <is>
           <t>aver</t>
         </is>
       </c>
-      <c r="C164" t="n">
-        <v>92908.28814911611</v>
-      </c>
-      <c r="D164" t="n">
-        <v>92908.28814911611</v>
+      <c r="C167" t="n">
+        <v>92908.36691466116</v>
+      </c>
+      <c r="D167" t="n">
+        <v>92908.495214721</v>
+      </c>
+      <c r="E167" t="n">
+        <v>92908.38829800449</v>
+      </c>
+      <c r="F167" t="n">
+        <v>92908.41680912887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>